<commit_message>
ajout charge selon la période
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clementrieux/Documents/workout_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1B82CDE-5157-EC43-BE20-1A6666494083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBF60C1-DA01-F04C-83E8-93C3F3B3CA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{062088F5-F1DE-C94A-B268-63A17544111A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>date</t>
   </si>
@@ -47,9 +47,6 @@
     <t>DC</t>
   </si>
   <si>
-    <t>squat</t>
-  </si>
-  <si>
     <t>serie</t>
   </si>
   <si>
@@ -57,6 +54,45 @@
   </si>
   <si>
     <t>charge (kg)</t>
+  </si>
+  <si>
+    <t>Snatch</t>
+  </si>
+  <si>
+    <t>Pull Over</t>
+  </si>
+  <si>
+    <t>52.5</t>
+  </si>
+  <si>
+    <t>Squat</t>
+  </si>
+  <si>
+    <t>Good morning</t>
+  </si>
+  <si>
+    <t>Mollet</t>
+  </si>
+  <si>
+    <t>Adducteur interne</t>
+  </si>
+  <si>
+    <t>Fessiers</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>Leg curl</t>
+  </si>
+  <si>
+    <t>Leg extension</t>
+  </si>
+  <si>
+    <t>Dev militaire</t>
+  </si>
+  <si>
+    <t>Dev nuque</t>
   </si>
 </sst>
 </file>
@@ -94,7 +130,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF27564-A964-DC42-8B25-2E776B819AB8}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,21 +461,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44896</v>
+        <v>44893</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -447,13 +483,13 @@
       <c r="D2">
         <v>5</v>
       </c>
-      <c r="E2">
-        <v>60</v>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44897</v>
+        <v>44893</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -465,32 +501,32 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44898</v>
+        <v>44893</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44899</v>
+        <v>44894</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -499,134 +535,134 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>75</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44900</v>
+        <v>44894</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E6">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44901</v>
+        <v>44894</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>80</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44902</v>
+        <v>44894</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>82</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44903</v>
+        <v>44894</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>82</v>
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44904</v>
+        <v>44894</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E10">
-        <v>85</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44905</v>
+        <v>44894</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44906</v>
+        <v>44895</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E12">
-        <v>90</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>44907</v>
+        <v>44895</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -635,24 +671,24 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <v>92</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>44908</v>
+        <v>44896</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E14">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -660,7 +696,7 @@
         <v>44896</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -669,15 +705,15 @@
         <v>5</v>
       </c>
       <c r="E15">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>44897</v>
+        <v>44900</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -685,16 +721,16 @@
       <c r="D16">
         <v>5</v>
       </c>
-      <c r="E16">
-        <v>90</v>
+      <c r="E16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>44898</v>
+        <v>44900</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -703,32 +739,32 @@
         <v>5</v>
       </c>
       <c r="E17">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>44899</v>
+        <v>44900</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>105</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>44900</v>
+        <v>44901</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -737,7 +773,7 @@
         <v>5</v>
       </c>
       <c r="E19">
-        <v>110</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -745,126 +781,126 @@
         <v>44901</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E20">
-        <v>120</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>44902</v>
+        <v>44901</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E21">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>44903</v>
+        <v>44901</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E22">
-        <v>145</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>44904</v>
+        <v>44901</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <v>150</v>
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>44905</v>
+        <v>44901</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C24">
         <v>4</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>155</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>44906</v>
+        <v>44901</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E25">
-        <v>160</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>44907</v>
+        <v>44902</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E26">
-        <v>165</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>44908</v>
+        <v>44902</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -873,7 +909,41 @@
         <v>3</v>
       </c>
       <c r="E27">
-        <v>170</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>44903</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>44903</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>